<commit_message>
Weekly backup - July 13, 2017
</commit_message>
<xml_diff>
--- a/wp-content/uploads/Ratecard_AdUX.xlsx
+++ b/wp-content/uploads/Ratecard_AdUX.xlsx
@@ -1012,12 +1012,6 @@
     <t>Démotivateur</t>
   </si>
   <si>
-    <t>CPM 70€</t>
-  </si>
-  <si>
-    <t>CPM 75€</t>
-  </si>
-  <si>
     <t>Campaign manager</t>
   </si>
   <si>
@@ -1064,6 +1058,12 @@
   </si>
   <si>
     <t>*100% SOV</t>
+  </si>
+  <si>
+    <t>CPM 50€</t>
+  </si>
+  <si>
+    <t>CPM 40€</t>
   </si>
 </sst>
 </file>
@@ -3161,9 +3161,6 @@
     <xf numFmtId="3" fontId="7" fillId="8" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -3326,6 +3323,90 @@
     <xf numFmtId="9" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="56" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="15" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="57" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="27" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="28" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="29" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="0" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="26" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="25" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3335,18 +3416,9 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="26" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="56" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="57" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="169" fontId="40" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3356,78 +3428,6 @@
     <xf numFmtId="169" fontId="40" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="27" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="28" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="29" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="9" borderId="0" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="9" borderId="26" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="15" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3440,6 +3440,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3452,83 +3473,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3554,59 +3587,32 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="26" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="26" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="26" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="8" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="8" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="8" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -3614,11 +3620,71 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="37" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="40" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3627,72 +3693,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="37" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="40" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4109,7 +4109,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4925,7 +4925,7 @@
         <xdr:cNvPr id="6" name="Image 5" descr="Résultat de recherche d'images pour &quot;microsoft nouveau logo png&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5868,7 +5868,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2F865116-8830-43AB-B730-E43892058C40}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F865116-8830-43AB-B730-E43892058C40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6698,7 +6698,7 @@
         <xdr:cNvPr id="17" name="Rectangle 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2F865116-8830-43AB-B730-E43892058C40}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F865116-8830-43AB-B730-E43892058C40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6769,7 +6769,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2" invalidUrl="http://hmbdoc.be/Docs/AdPulse Content.pptx"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C11164FB-82E4-4FB2-A9D4-FF64A5F2A9E5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C11164FB-82E4-4FB2-A9D4-FF64A5F2A9E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9216,6 +9216,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>209549</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rectangle 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000125" y="5219700"/>
+          <a:ext cx="2952751" cy="638174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F58226"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="F58226"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-BE" sz="1100" b="1">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>+25%</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-BE" sz="1100" b="1" baseline="0">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t> targeting</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-BE" sz="1100" b="1">
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9497,7 +9573,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="Résultat de recherche d'images pour &quot;microsoft nouveau logo png&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9961,7 +10037,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="Résultat de recherche d'images pour &quot;microsoft nouveau logo png&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12252,84 +12328,84 @@
   <sheetData>
     <row r="1" spans="2:8" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="206"/>
-      <c r="C2" s="209" t="s">
-        <v>325</v>
-      </c>
-      <c r="D2" s="209"/>
-      <c r="E2" s="209"/>
-      <c r="F2" s="209"/>
-      <c r="G2" s="209"/>
-      <c r="H2" s="210"/>
+      <c r="B2" s="195"/>
+      <c r="C2" s="198" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="199"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="207"/>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
-      <c r="H3" s="212"/>
+      <c r="B3" s="196"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="201"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="207"/>
-      <c r="C4" s="211"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="212"/>
+      <c r="B4" s="196"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="200"/>
+      <c r="H4" s="201"/>
     </row>
     <row r="5" spans="2:8" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="208"/>
-      <c r="C5" s="213"/>
-      <c r="D5" s="213"/>
-      <c r="E5" s="213"/>
-      <c r="F5" s="213"/>
-      <c r="G5" s="213"/>
-      <c r="H5" s="214"/>
+      <c r="B5" s="197"/>
+      <c r="C5" s="202"/>
+      <c r="D5" s="202"/>
+      <c r="E5" s="202"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="203"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="215"/>
-      <c r="C6" s="216"/>
-      <c r="D6" s="216"/>
-      <c r="E6" s="216"/>
-      <c r="F6" s="216"/>
-      <c r="G6" s="216"/>
-      <c r="H6" s="217"/>
+      <c r="B6" s="204"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
+      <c r="G6" s="205"/>
+      <c r="H6" s="206"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="190" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195"/>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195"/>
-      <c r="H7" s="196"/>
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="194"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="218"/>
-      <c r="C8" s="219"/>
-      <c r="D8" s="220"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="219"/>
-      <c r="G8" s="219"/>
-      <c r="H8" s="221"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="208"/>
+      <c r="D8" s="209"/>
+      <c r="E8" s="208"/>
+      <c r="F8" s="208"/>
+      <c r="G8" s="208"/>
+      <c r="H8" s="210"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="193" t="s">
+      <c r="B9" s="190" t="s">
         <v>260</v>
       </c>
-      <c r="C9" s="222"/>
+      <c r="C9" s="191"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="223" t="s">
+      <c r="E9" s="192" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="195"/>
-      <c r="G9" s="195"/>
-      <c r="H9" s="196"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="194"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="78"/>
@@ -12348,11 +12424,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D11" s="15"/>
-      <c r="E11" s="203" t="s">
+      <c r="E11" s="214" t="s">
         <v>137</v>
       </c>
-      <c r="F11" s="203"/>
-      <c r="G11" s="189" t="s">
+      <c r="F11" s="214"/>
+      <c r="G11" s="188" t="s">
         <v>56</v>
       </c>
       <c r="H11" s="80"/>
@@ -12365,11 +12441,11 @@
         <v>0.05</v>
       </c>
       <c r="D12" s="16"/>
-      <c r="E12" s="203" t="s">
+      <c r="E12" s="214" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="203"/>
-      <c r="G12" s="189">
+      <c r="F12" s="214"/>
+      <c r="G12" s="188">
         <v>0.25</v>
       </c>
       <c r="H12" s="80"/>
@@ -12382,11 +12458,11 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D13" s="15"/>
-      <c r="E13" s="203" t="s">
+      <c r="E13" s="214" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="203"/>
-      <c r="G13" s="189">
+      <c r="F13" s="214"/>
+      <c r="G13" s="188">
         <v>0.25</v>
       </c>
       <c r="H13" s="80"/>
@@ -12399,11 +12475,11 @@
         <v>0.1</v>
       </c>
       <c r="D14" s="16"/>
-      <c r="E14" s="203" t="s">
+      <c r="E14" s="214" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="203"/>
-      <c r="G14" s="189">
+      <c r="F14" s="214"/>
+      <c r="G14" s="188">
         <v>0.5</v>
       </c>
       <c r="H14" s="80"/>
@@ -12416,11 +12492,11 @@
         <v>0.125</v>
       </c>
       <c r="D15" s="15"/>
-      <c r="E15" s="203" t="s">
+      <c r="E15" s="214" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="203"/>
-      <c r="G15" s="189">
+      <c r="F15" s="214"/>
+      <c r="G15" s="188">
         <v>0.15</v>
       </c>
       <c r="H15" s="80"/>
@@ -12461,12 +12537,12 @@
         <v>0.2</v>
       </c>
       <c r="D18" s="16"/>
-      <c r="E18" s="204" t="s">
+      <c r="E18" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="204"/>
-      <c r="G18" s="204"/>
-      <c r="H18" s="205"/>
+      <c r="F18" s="215"/>
+      <c r="G18" s="215"/>
+      <c r="H18" s="216"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="30" t="s">
@@ -12476,10 +12552,10 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="D19" s="15"/>
-      <c r="E19" s="204"/>
-      <c r="F19" s="204"/>
-      <c r="G19" s="204"/>
-      <c r="H19" s="205"/>
+      <c r="E19" s="215"/>
+      <c r="F19" s="215"/>
+      <c r="G19" s="215"/>
+      <c r="H19" s="216"/>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="30" t="s">
@@ -12528,15 +12604,15 @@
       <c r="H23" s="80"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="190" t="s">
+      <c r="B24" s="217" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="191"/>
-      <c r="D24" s="191"/>
-      <c r="E24" s="191"/>
-      <c r="F24" s="191"/>
-      <c r="G24" s="191"/>
-      <c r="H24" s="192"/>
+      <c r="C24" s="218"/>
+      <c r="D24" s="218"/>
+      <c r="E24" s="218"/>
+      <c r="F24" s="218"/>
+      <c r="G24" s="218"/>
+      <c r="H24" s="219"/>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="82"/>
@@ -12602,15 +12678,15 @@
       <c r="H29" s="80"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="193" t="s">
+      <c r="B30" s="190" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="194"/>
-      <c r="D30" s="195"/>
-      <c r="E30" s="194"/>
-      <c r="F30" s="195"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="196"/>
+      <c r="C30" s="220"/>
+      <c r="D30" s="193"/>
+      <c r="E30" s="220"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="194"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="84"/>
@@ -12622,15 +12698,15 @@
       <c r="H31" s="85"/>
     </row>
     <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="197" t="s">
+      <c r="B32" s="221" t="s">
         <v>294</v>
       </c>
-      <c r="C32" s="198"/>
-      <c r="D32" s="198"/>
-      <c r="E32" s="198"/>
-      <c r="F32" s="198"/>
-      <c r="G32" s="198"/>
-      <c r="H32" s="199"/>
+      <c r="C32" s="222"/>
+      <c r="D32" s="222"/>
+      <c r="E32" s="222"/>
+      <c r="F32" s="222"/>
+      <c r="G32" s="222"/>
+      <c r="H32" s="223"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="84"/>
@@ -12898,34 +12974,34 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="83" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G49" s="23"/>
       <c r="H49" s="87"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="83" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F50" s="21" t="s">
         <v>321</v>
-      </c>
-      <c r="F50" s="21" t="s">
-        <v>323</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="87"/>
@@ -12940,15 +13016,15 @@
       <c r="H51" s="85"/>
     </row>
     <row r="52" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="197" t="s">
+      <c r="B52" s="221" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="198"/>
-      <c r="D52" s="198"/>
-      <c r="E52" s="198"/>
-      <c r="F52" s="198"/>
-      <c r="G52" s="198"/>
-      <c r="H52" s="199"/>
+      <c r="C52" s="222"/>
+      <c r="D52" s="222"/>
+      <c r="E52" s="222"/>
+      <c r="F52" s="222"/>
+      <c r="G52" s="222"/>
+      <c r="H52" s="223"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="84"/>
@@ -13047,15 +13123,15 @@
       <c r="H60" s="85"/>
     </row>
     <row r="61" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="197" t="s">
+      <c r="B61" s="221" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="198"/>
-      <c r="D61" s="198"/>
-      <c r="E61" s="198"/>
-      <c r="F61" s="198"/>
-      <c r="G61" s="198"/>
-      <c r="H61" s="199"/>
+      <c r="C61" s="222"/>
+      <c r="D61" s="222"/>
+      <c r="E61" s="222"/>
+      <c r="F61" s="222"/>
+      <c r="G61" s="222"/>
+      <c r="H61" s="223"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="84"/>
@@ -13240,25 +13316,18 @@
       <c r="H77" s="93"/>
     </row>
     <row r="78" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="200" t="s">
+      <c r="B78" s="211" t="s">
         <v>170</v>
       </c>
-      <c r="C78" s="201"/>
-      <c r="D78" s="201"/>
-      <c r="E78" s="201"/>
-      <c r="F78" s="201"/>
-      <c r="G78" s="201"/>
-      <c r="H78" s="202"/>
+      <c r="C78" s="212"/>
+      <c r="D78" s="212"/>
+      <c r="E78" s="212"/>
+      <c r="F78" s="212"/>
+      <c r="G78" s="212"/>
+      <c r="H78" s="213"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
     <mergeCell ref="B78:H78"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
@@ -13271,6 +13340,13 @@
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B52:H52"/>
     <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C54" r:id="rId1"/>
@@ -13326,16 +13402,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="141"/>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="143"/>
+      <c r="A1" s="140"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="142"/>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
@@ -13904,32 +13980,32 @@
   <sheetData>
     <row r="1" spans="2:8" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="144"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="146"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="145"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="63"/>
-      <c r="C3" s="292" t="s">
+      <c r="C3" s="288" t="s">
         <v>303</v>
       </c>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="294"/>
+      <c r="D3" s="289"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="289"/>
+      <c r="G3" s="290"/>
       <c r="H3" s="64"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="63"/>
-      <c r="C4" s="295"/>
-      <c r="D4" s="296"/>
-      <c r="E4" s="296"/>
-      <c r="F4" s="296"/>
-      <c r="G4" s="297"/>
+      <c r="C4" s="291"/>
+      <c r="D4" s="292"/>
+      <c r="E4" s="292"/>
+      <c r="F4" s="292"/>
+      <c r="G4" s="293"/>
       <c r="H4" s="64"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -13952,10 +14028,10 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="63"/>
-      <c r="C7" s="311" t="s">
+      <c r="C7" s="308" t="s">
         <v>244</v>
       </c>
-      <c r="D7" s="312"/>
+      <c r="D7" s="309"/>
       <c r="E7" s="61" t="s">
         <v>240</v>
       </c>
@@ -13969,66 +14045,66 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="63"/>
-      <c r="C8" s="302"/>
-      <c r="D8" s="305"/>
-      <c r="E8" s="307" t="s">
+      <c r="C8" s="299"/>
+      <c r="D8" s="302"/>
+      <c r="E8" s="304" t="s">
         <v>243</v>
       </c>
-      <c r="F8" s="307" t="s">
+      <c r="F8" s="304" t="s">
         <v>250</v>
       </c>
-      <c r="G8" s="288">
+      <c r="G8" s="310">
         <v>1.63</v>
       </c>
       <c r="H8" s="64"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="63"/>
-      <c r="C9" s="303"/>
-      <c r="D9" s="306"/>
-      <c r="E9" s="308"/>
-      <c r="F9" s="308"/>
-      <c r="G9" s="289"/>
+      <c r="C9" s="300"/>
+      <c r="D9" s="303"/>
+      <c r="E9" s="305"/>
+      <c r="F9" s="305"/>
+      <c r="G9" s="311"/>
       <c r="H9" s="64"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="63"/>
-      <c r="C10" s="303"/>
-      <c r="D10" s="306"/>
-      <c r="E10" s="309"/>
-      <c r="F10" s="309"/>
-      <c r="G10" s="289"/>
+      <c r="C10" s="300"/>
+      <c r="D10" s="303"/>
+      <c r="E10" s="306"/>
+      <c r="F10" s="306"/>
+      <c r="G10" s="311"/>
       <c r="H10" s="64"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="63"/>
-      <c r="C11" s="303"/>
-      <c r="D11" s="306"/>
-      <c r="E11" s="308" t="s">
+      <c r="C11" s="300"/>
+      <c r="D11" s="303"/>
+      <c r="E11" s="305" t="s">
         <v>242</v>
       </c>
-      <c r="F11" s="308" t="s">
+      <c r="F11" s="305" t="s">
         <v>251</v>
       </c>
-      <c r="G11" s="289"/>
+      <c r="G11" s="311"/>
       <c r="H11" s="64"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="63"/>
-      <c r="C12" s="303"/>
-      <c r="D12" s="306"/>
-      <c r="E12" s="308"/>
-      <c r="F12" s="308"/>
-      <c r="G12" s="289"/>
+      <c r="C12" s="300"/>
+      <c r="D12" s="303"/>
+      <c r="E12" s="305"/>
+      <c r="F12" s="305"/>
+      <c r="G12" s="311"/>
       <c r="H12" s="64"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="63"/>
-      <c r="C13" s="304"/>
-      <c r="D13" s="182"/>
-      <c r="E13" s="310"/>
-      <c r="F13" s="310"/>
-      <c r="G13" s="290"/>
+      <c r="C13" s="301"/>
+      <c r="D13" s="181"/>
+      <c r="E13" s="307"/>
+      <c r="F13" s="307"/>
+      <c r="G13" s="312"/>
       <c r="H13" s="64"/>
     </row>
     <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14042,13 +14118,13 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="63"/>
-      <c r="C15" s="300" t="s">
+      <c r="C15" s="297" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="301"/>
-      <c r="E15" s="301"/>
-      <c r="F15" s="301"/>
-      <c r="G15" s="301"/>
+      <c r="D15" s="298"/>
+      <c r="E15" s="298"/>
+      <c r="F15" s="298"/>
+      <c r="G15" s="298"/>
       <c r="H15" s="64"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -14062,123 +14138,123 @@
     </row>
     <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="63"/>
-      <c r="C17" s="298" t="s">
+      <c r="C17" s="294" t="s">
         <v>245</v>
       </c>
-      <c r="D17" s="298"/>
-      <c r="E17" s="298"/>
-      <c r="F17" s="298"/>
-      <c r="G17" s="298"/>
+      <c r="D17" s="294"/>
+      <c r="E17" s="294"/>
+      <c r="F17" s="294"/>
+      <c r="G17" s="294"/>
       <c r="H17" s="65"/>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="63"/>
-      <c r="C18" s="291" t="s">
+      <c r="C18" s="295" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="291"/>
-      <c r="E18" s="291"/>
-      <c r="F18" s="291"/>
-      <c r="G18" s="291"/>
+      <c r="D18" s="295"/>
+      <c r="E18" s="295"/>
+      <c r="F18" s="295"/>
+      <c r="G18" s="295"/>
       <c r="H18" s="65"/>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="63"/>
-      <c r="C19" s="291" t="s">
+      <c r="C19" s="295" t="s">
         <v>256</v>
       </c>
-      <c r="D19" s="291"/>
-      <c r="E19" s="291"/>
-      <c r="F19" s="291"/>
-      <c r="G19" s="291"/>
+      <c r="D19" s="295"/>
+      <c r="E19" s="295"/>
+      <c r="F19" s="295"/>
+      <c r="G19" s="295"/>
       <c r="H19" s="65"/>
     </row>
     <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="63"/>
-      <c r="C20" s="291" t="s">
+      <c r="C20" s="295" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="291"/>
-      <c r="E20" s="291"/>
-      <c r="F20" s="291"/>
-      <c r="G20" s="291"/>
+      <c r="D20" s="295"/>
+      <c r="E20" s="295"/>
+      <c r="F20" s="295"/>
+      <c r="G20" s="295"/>
       <c r="H20" s="65"/>
     </row>
     <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="63"/>
-      <c r="C21" s="291" t="s">
+      <c r="C21" s="295" t="s">
         <v>223</v>
       </c>
-      <c r="D21" s="291"/>
-      <c r="E21" s="291"/>
-      <c r="F21" s="291"/>
-      <c r="G21" s="291"/>
+      <c r="D21" s="295"/>
+      <c r="E21" s="295"/>
+      <c r="F21" s="295"/>
+      <c r="G21" s="295"/>
       <c r="H21" s="65"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="63"/>
-      <c r="C22" s="291" t="s">
+      <c r="C22" s="295" t="s">
         <v>224</v>
       </c>
-      <c r="D22" s="291"/>
-      <c r="E22" s="291"/>
-      <c r="F22" s="291"/>
-      <c r="G22" s="291"/>
+      <c r="D22" s="295"/>
+      <c r="E22" s="295"/>
+      <c r="F22" s="295"/>
+      <c r="G22" s="295"/>
       <c r="H22" s="65"/>
     </row>
     <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="63"/>
-      <c r="C23" s="298" t="s">
+      <c r="C23" s="294" t="s">
         <v>126</v>
       </c>
-      <c r="D23" s="298"/>
-      <c r="E23" s="298"/>
-      <c r="F23" s="298"/>
-      <c r="G23" s="298"/>
+      <c r="D23" s="294"/>
+      <c r="E23" s="294"/>
+      <c r="F23" s="294"/>
+      <c r="G23" s="294"/>
       <c r="H23" s="65"/>
     </row>
     <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="63"/>
-      <c r="C24" s="291" t="s">
+      <c r="C24" s="295" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="291"/>
-      <c r="E24" s="291"/>
-      <c r="F24" s="291"/>
-      <c r="G24" s="291"/>
+      <c r="D24" s="295"/>
+      <c r="E24" s="295"/>
+      <c r="F24" s="295"/>
+      <c r="G24" s="295"/>
       <c r="H24" s="65"/>
     </row>
     <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="63"/>
-      <c r="C25" s="299" t="s">
+      <c r="C25" s="296" t="s">
         <v>174</v>
       </c>
-      <c r="D25" s="299"/>
-      <c r="E25" s="299"/>
-      <c r="F25" s="299"/>
-      <c r="G25" s="299"/>
+      <c r="D25" s="296"/>
+      <c r="E25" s="296"/>
+      <c r="F25" s="296"/>
+      <c r="G25" s="296"/>
       <c r="H25" s="68"/>
     </row>
     <row r="26" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="63"/>
-      <c r="C26" s="299" t="s">
+      <c r="C26" s="296" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="299"/>
-      <c r="E26" s="299"/>
-      <c r="F26" s="299"/>
-      <c r="G26" s="299"/>
+      <c r="D26" s="296"/>
+      <c r="E26" s="296"/>
+      <c r="F26" s="296"/>
+      <c r="G26" s="296"/>
       <c r="H26" s="68"/>
     </row>
     <row r="27" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="63"/>
-      <c r="C27" s="291" t="s">
+      <c r="C27" s="295" t="s">
         <v>304</v>
       </c>
-      <c r="D27" s="291"/>
-      <c r="E27" s="291"/>
-      <c r="F27" s="291"/>
-      <c r="G27" s="291"/>
+      <c r="D27" s="295"/>
+      <c r="E27" s="295"/>
+      <c r="F27" s="295"/>
+      <c r="G27" s="295"/>
       <c r="H27" s="69"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14192,6 +14268,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="C24:G24"/>
@@ -14208,12 +14290,6 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14226,7 +14302,7 @@
   <dimension ref="B1:W32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14351,44 +14427,44 @@
     </row>
     <row r="6" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="36"/>
-      <c r="C6" s="234" t="s">
+      <c r="C6" s="230" t="s">
         <v>291</v>
       </c>
-      <c r="D6" s="235"/>
-      <c r="E6" s="236" t="s">
+      <c r="D6" s="231"/>
+      <c r="E6" s="232" t="s">
         <v>220</v>
       </c>
-      <c r="F6" s="237"/>
-      <c r="G6" s="236" t="s">
+      <c r="F6" s="233"/>
+      <c r="G6" s="232" t="s">
         <v>290</v>
       </c>
-      <c r="H6" s="238"/>
+      <c r="H6" s="234"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="234" t="s">
+      <c r="J6" s="230" t="s">
         <v>292</v>
       </c>
-      <c r="K6" s="235"/>
-      <c r="L6" s="232" t="s">
+      <c r="K6" s="231"/>
+      <c r="L6" s="228" t="s">
         <v>219</v>
       </c>
-      <c r="M6" s="233"/>
-      <c r="N6" s="236" t="s">
+      <c r="M6" s="229"/>
+      <c r="N6" s="232" t="s">
         <v>290</v>
       </c>
-      <c r="O6" s="238"/>
+      <c r="O6" s="234"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="234" t="s">
+      <c r="Q6" s="230" t="s">
         <v>293</v>
       </c>
-      <c r="R6" s="235"/>
-      <c r="S6" s="232" t="s">
+      <c r="R6" s="231"/>
+      <c r="S6" s="228" t="s">
         <v>219</v>
       </c>
-      <c r="T6" s="233"/>
-      <c r="U6" s="232" t="s">
+      <c r="T6" s="229"/>
+      <c r="U6" s="228" t="s">
         <v>290</v>
       </c>
-      <c r="V6" s="233"/>
+      <c r="V6" s="229"/>
       <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14751,14 +14827,14 @@
         <v>12321</v>
       </c>
       <c r="P14" s="10"/>
-      <c r="Q14" s="234" t="s">
+      <c r="Q14" s="230" t="s">
         <v>237</v>
       </c>
-      <c r="R14" s="235"/>
-      <c r="S14" s="232" t="s">
+      <c r="R14" s="231"/>
+      <c r="S14" s="228" t="s">
         <v>219</v>
       </c>
-      <c r="T14" s="233"/>
+      <c r="T14" s="229"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="37"/>
@@ -14924,8 +15000,8 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="228"/>
-      <c r="K19" s="229"/>
+      <c r="J19" s="235"/>
+      <c r="K19" s="236"/>
       <c r="L19" s="114" t="s">
         <v>141</v>
       </c>
@@ -14956,8 +15032,8 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="230"/>
-      <c r="K20" s="231"/>
+      <c r="J20" s="237"/>
+      <c r="K20" s="238"/>
       <c r="L20" s="115" t="s">
         <v>184</v>
       </c>
@@ -14988,8 +15064,8 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="228"/>
-      <c r="K21" s="229"/>
+      <c r="J21" s="235"/>
+      <c r="K21" s="236"/>
       <c r="L21" s="114" t="s">
         <v>141</v>
       </c>
@@ -15020,8 +15096,8 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="230"/>
-      <c r="K22" s="231"/>
+      <c r="J22" s="237"/>
+      <c r="K22" s="238"/>
       <c r="L22" s="115" t="s">
         <v>184</v>
       </c>
@@ -15084,14 +15160,14 @@
       <c r="M24" s="39"/>
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
-      <c r="P24" s="183"/>
-      <c r="Q24" s="183"/>
-      <c r="R24" s="183"/>
-      <c r="S24" s="183"/>
-      <c r="T24" s="183"/>
+      <c r="P24" s="182"/>
+      <c r="Q24" s="182"/>
+      <c r="R24" s="182"/>
+      <c r="S24" s="182"/>
+      <c r="T24" s="182"/>
       <c r="U24" s="39"/>
-      <c r="V24" s="183"/>
-      <c r="W24" s="184" t="s">
+      <c r="V24" s="182"/>
+      <c r="W24" s="183" t="s">
         <v>170</v>
       </c>
     </row>
@@ -15105,11 +15181,13 @@
     <row r="32" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="J15:K16"/>
-    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="J21:K22"/>
+    <mergeCell ref="J19:K20"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="J13:K14"/>
+    <mergeCell ref="Q15:R16"/>
+    <mergeCell ref="J17:K18"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="S14:T14"/>
@@ -15126,13 +15204,11 @@
     <mergeCell ref="Q7:R8"/>
     <mergeCell ref="C11:D12"/>
     <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="J21:K22"/>
-    <mergeCell ref="J19:K20"/>
-    <mergeCell ref="J11:K12"/>
-    <mergeCell ref="J13:K14"/>
-    <mergeCell ref="Q15:R16"/>
-    <mergeCell ref="J17:K18"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="J15:K16"/>
+    <mergeCell ref="J9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15461,7 +15537,7 @@
       <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="140"/>
+      <c r="A20" s="139"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -15511,8 +15587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15637,50 +15713,50 @@
     </row>
     <row r="6" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="36"/>
-      <c r="C6" s="234" t="s">
+      <c r="C6" s="230" t="s">
         <v>295</v>
       </c>
-      <c r="D6" s="235"/>
-      <c r="E6" s="236" t="s">
-        <v>316</v>
-      </c>
-      <c r="F6" s="237"/>
-      <c r="G6" s="236" t="s">
-        <v>326</v>
-      </c>
-      <c r="H6" s="238"/>
+      <c r="D6" s="231"/>
+      <c r="E6" s="232" t="s">
+        <v>327</v>
+      </c>
+      <c r="F6" s="233"/>
+      <c r="G6" s="232" t="s">
+        <v>324</v>
+      </c>
+      <c r="H6" s="234"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="234" t="s">
+      <c r="J6" s="230" t="s">
         <v>296</v>
       </c>
-      <c r="K6" s="235"/>
-      <c r="L6" s="243" t="s">
-        <v>297</v>
-      </c>
-      <c r="M6" s="244"/>
-      <c r="N6" s="236" t="s">
-        <v>326</v>
-      </c>
-      <c r="O6" s="238"/>
+      <c r="K6" s="231"/>
+      <c r="L6" s="241" t="s">
+        <v>220</v>
+      </c>
+      <c r="M6" s="242"/>
+      <c r="N6" s="232" t="s">
+        <v>324</v>
+      </c>
+      <c r="O6" s="234"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="234" t="s">
+      <c r="Q6" s="230" t="s">
         <v>264</v>
       </c>
-      <c r="R6" s="235"/>
-      <c r="S6" s="232" t="s">
-        <v>297</v>
-      </c>
-      <c r="T6" s="233"/>
-      <c r="U6" s="236" t="s">
-        <v>326</v>
-      </c>
-      <c r="V6" s="238"/>
+      <c r="R6" s="231"/>
+      <c r="S6" s="228" t="s">
+        <v>328</v>
+      </c>
+      <c r="T6" s="229"/>
+      <c r="U6" s="232" t="s">
+        <v>324</v>
+      </c>
+      <c r="V6" s="234"/>
       <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36"/>
       <c r="C7" s="224"/>
-      <c r="D7" s="241"/>
+      <c r="D7" s="247"/>
       <c r="E7" s="114" t="s">
         <v>141</v>
       </c>
@@ -15728,7 +15804,7 @@
     <row r="8" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="36"/>
       <c r="C8" s="226"/>
-      <c r="D8" s="242"/>
+      <c r="D8" s="248"/>
       <c r="E8" s="115" t="s">
         <v>184</v>
       </c>
@@ -15776,7 +15852,7 @@
     <row r="9" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="36"/>
       <c r="C9" s="224"/>
-      <c r="D9" s="241"/>
+      <c r="D9" s="247"/>
       <c r="E9" s="114" t="s">
         <v>141</v>
       </c>
@@ -15824,7 +15900,7 @@
     <row r="10" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="36"/>
       <c r="C10" s="226"/>
-      <c r="D10" s="242"/>
+      <c r="D10" s="248"/>
       <c r="E10" s="115" t="s">
         <v>184</v>
       </c>
@@ -15872,7 +15948,7 @@
     <row r="11" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="36"/>
       <c r="C11" s="224"/>
-      <c r="D11" s="241"/>
+      <c r="D11" s="247"/>
       <c r="E11" s="114" t="s">
         <v>141</v>
       </c>
@@ -15920,7 +15996,7 @@
     <row r="12" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="36"/>
       <c r="C12" s="226"/>
-      <c r="D12" s="242"/>
+      <c r="D12" s="248"/>
       <c r="E12" s="115" t="s">
         <v>184</v>
       </c>
@@ -15968,7 +16044,7 @@
     <row r="13" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="36"/>
       <c r="C13" s="224"/>
-      <c r="D13" s="241"/>
+      <c r="D13" s="247"/>
       <c r="E13" s="114" t="s">
         <v>141</v>
       </c>
@@ -16008,7 +16084,7 @@
     <row r="14" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="36"/>
       <c r="C14" s="226"/>
-      <c r="D14" s="242"/>
+      <c r="D14" s="248"/>
       <c r="E14" s="115" t="s">
         <v>184</v>
       </c>
@@ -16048,7 +16124,7 @@
     <row r="15" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="36"/>
       <c r="C15" s="224"/>
-      <c r="D15" s="241"/>
+      <c r="D15" s="247"/>
       <c r="E15" s="114" t="s">
         <v>141</v>
       </c>
@@ -16077,24 +16153,24 @@
         <v>1346</v>
       </c>
       <c r="P15" s="10"/>
-      <c r="Q15" s="234" t="s">
-        <v>327</v>
-      </c>
-      <c r="R15" s="235"/>
-      <c r="S15" s="232" t="s">
-        <v>317</v>
-      </c>
-      <c r="T15" s="233"/>
-      <c r="U15" s="236" t="s">
-        <v>326</v>
-      </c>
-      <c r="V15" s="238"/>
+      <c r="Q15" s="230" t="s">
+        <v>325</v>
+      </c>
+      <c r="R15" s="231"/>
+      <c r="S15" s="228" t="s">
+        <v>297</v>
+      </c>
+      <c r="T15" s="229"/>
+      <c r="U15" s="232" t="s">
+        <v>324</v>
+      </c>
+      <c r="V15" s="234"/>
       <c r="W15" s="37"/>
     </row>
     <row r="16" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36"/>
       <c r="C16" s="226"/>
-      <c r="D16" s="242"/>
+      <c r="D16" s="248"/>
       <c r="E16" s="115" t="s">
         <v>184</v>
       </c>
@@ -16308,8 +16384,8 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="228"/>
-      <c r="K21" s="229"/>
+      <c r="J21" s="235"/>
+      <c r="K21" s="236"/>
       <c r="L21" s="114" t="s">
         <v>141</v>
       </c>
@@ -16348,8 +16424,8 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="230"/>
-      <c r="K22" s="231"/>
+      <c r="J22" s="237"/>
+      <c r="K22" s="238"/>
       <c r="L22" s="115" t="s">
         <v>184</v>
       </c>
@@ -16388,8 +16464,8 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="228"/>
-      <c r="K23" s="229"/>
+      <c r="J23" s="235"/>
+      <c r="K23" s="236"/>
       <c r="L23" s="114" t="s">
         <v>141</v>
       </c>
@@ -16428,8 +16504,8 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="230"/>
-      <c r="K24" s="231"/>
+      <c r="J24" s="237"/>
+      <c r="K24" s="238"/>
       <c r="L24" s="115" t="s">
         <v>184</v>
       </c>
@@ -16699,8 +16775,8 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
-      <c r="Q32" s="228"/>
-      <c r="R32" s="229"/>
+      <c r="Q32" s="235"/>
+      <c r="R32" s="236"/>
       <c r="S32" s="114" t="s">
         <v>141</v>
       </c>
@@ -16731,8 +16807,8 @@
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
-      <c r="Q33" s="230"/>
-      <c r="R33" s="231"/>
+      <c r="Q33" s="237"/>
+      <c r="R33" s="238"/>
       <c r="S33" s="115" t="s">
         <v>184</v>
       </c>
@@ -16964,11 +17040,11 @@
       <c r="W40" s="37"/>
     </row>
     <row r="41" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="245" t="s">
-        <v>328</v>
-      </c>
-      <c r="C41" s="246"/>
-      <c r="D41" s="246"/>
+      <c r="B41" s="243" t="s">
+        <v>326</v>
+      </c>
+      <c r="C41" s="244"/>
+      <c r="D41" s="244"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -16990,11 +17066,11 @@
       <c r="W41" s="37"/>
     </row>
     <row r="42" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="247"/>
-      <c r="C42" s="248"/>
-      <c r="D42" s="248"/>
-      <c r="E42" s="127"/>
-      <c r="F42" s="127"/>
+      <c r="B42" s="245"/>
+      <c r="C42" s="246"/>
+      <c r="D42" s="246"/>
+      <c r="E42" s="189"/>
+      <c r="F42" s="189"/>
       <c r="G42" s="39"/>
       <c r="H42" s="39"/>
       <c r="I42" s="239" t="s">
@@ -17017,6 +17093,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="J13:K14"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="J15:K16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="Q30:R31"/>
+    <mergeCell ref="Q16:R17"/>
+    <mergeCell ref="Q38:R39"/>
+    <mergeCell ref="J23:K24"/>
+    <mergeCell ref="Q36:R37"/>
+    <mergeCell ref="Q20:R21"/>
+    <mergeCell ref="Q32:R33"/>
+    <mergeCell ref="Q34:R35"/>
+    <mergeCell ref="J19:K20"/>
+    <mergeCell ref="Q28:R29"/>
+    <mergeCell ref="J21:K22"/>
+    <mergeCell ref="Q22:R23"/>
+    <mergeCell ref="Q24:R25"/>
+    <mergeCell ref="Q26:R27"/>
+    <mergeCell ref="Q18:R19"/>
+    <mergeCell ref="J17:K18"/>
     <mergeCell ref="I42:W42"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="J6:K6"/>
@@ -17033,33 +17136,6 @@
     <mergeCell ref="Q7:R8"/>
     <mergeCell ref="Q9:R10"/>
     <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="Q30:R31"/>
-    <mergeCell ref="Q16:R17"/>
-    <mergeCell ref="Q38:R39"/>
-    <mergeCell ref="J23:K24"/>
-    <mergeCell ref="Q36:R37"/>
-    <mergeCell ref="Q20:R21"/>
-    <mergeCell ref="Q32:R33"/>
-    <mergeCell ref="Q34:R35"/>
-    <mergeCell ref="J19:K20"/>
-    <mergeCell ref="Q28:R29"/>
-    <mergeCell ref="J21:K22"/>
-    <mergeCell ref="Q22:R23"/>
-    <mergeCell ref="Q24:R25"/>
-    <mergeCell ref="Q26:R27"/>
-    <mergeCell ref="Q18:R19"/>
-    <mergeCell ref="J17:K18"/>
-    <mergeCell ref="J15:K16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="J9:K10"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="J13:K14"/>
-    <mergeCell ref="J11:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17086,7 +17162,7 @@
   <sheetData>
     <row r="1" spans="2:16" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="188" t="s">
+      <c r="B2" s="187" t="s">
         <v>306</v>
       </c>
       <c r="C2" s="34"/>
@@ -17100,7 +17176,7 @@
       <c r="K2" s="35"/>
     </row>
     <row r="3" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="152" t="s">
+      <c r="B3" s="151" t="s">
         <v>308</v>
       </c>
       <c r="C3" s="10"/>
@@ -17118,8 +17194,8 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="254"/>
-      <c r="G4" s="254"/>
+      <c r="F4" s="249"/>
+      <c r="G4" s="249"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -17131,7 +17207,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="186"/>
+      <c r="G5" s="185"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -17139,13 +17215,13 @@
     </row>
     <row r="6" spans="2:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36"/>
-      <c r="C6" s="256" t="s">
+      <c r="C6" s="253" t="s">
         <v>261</v>
       </c>
-      <c r="D6" s="256"/>
-      <c r="E6" s="256"/>
-      <c r="F6" s="256"/>
-      <c r="G6" s="257"/>
+      <c r="D6" s="253"/>
+      <c r="E6" s="253"/>
+      <c r="F6" s="253"/>
+      <c r="G6" s="254"/>
       <c r="H6" s="120" t="s">
         <v>305</v>
       </c>
@@ -17159,26 +17235,26 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="36"/>
-      <c r="C7" s="255" t="s">
+      <c r="C7" s="250" t="s">
         <v>234</v>
       </c>
-      <c r="D7" s="255"/>
-      <c r="E7" s="147" t="s">
+      <c r="D7" s="250"/>
+      <c r="E7" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="147" t="s">
+      <c r="F7" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="148" t="s">
+      <c r="G7" s="147" t="s">
         <v>141</v>
       </c>
-      <c r="H7" s="149">
+      <c r="H7" s="148">
         <v>20</v>
       </c>
-      <c r="I7" s="150">
+      <c r="I7" s="149">
         <v>25</v>
       </c>
-      <c r="J7" s="151">
+      <c r="J7" s="150">
         <v>35</v>
       </c>
       <c r="K7" s="37"/>
@@ -17189,10 +17265,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="251"/>
-      <c r="E8" s="250" t="s">
+      <c r="E8" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F8" s="250"/>
+      <c r="F8" s="255"/>
       <c r="G8" s="41">
         <v>1600000</v>
       </c>
@@ -17209,14 +17285,14 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="36"/>
-      <c r="C9" s="249" t="s">
+      <c r="C9" s="252" t="s">
         <v>255</v>
       </c>
-      <c r="D9" s="249"/>
-      <c r="E9" s="185">
+      <c r="D9" s="252"/>
+      <c r="E9" s="184">
         <v>0.86</v>
       </c>
-      <c r="F9" s="185">
+      <c r="F9" s="184">
         <v>0.14000000000000001</v>
       </c>
       <c r="G9" s="41">
@@ -17232,7 +17308,7 @@
         <v>115500</v>
       </c>
       <c r="K9" s="37"/>
-      <c r="P9" s="187"/>
+      <c r="P9" s="186"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="36"/>
@@ -17240,10 +17316,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="251"/>
-      <c r="E10" s="250" t="s">
+      <c r="E10" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="250"/>
+      <c r="F10" s="255"/>
       <c r="G10" s="41">
         <v>1411349</v>
       </c>
@@ -17264,10 +17340,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="251"/>
-      <c r="E11" s="250" t="s">
+      <c r="E11" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="250"/>
+      <c r="F11" s="255"/>
       <c r="G11" s="41">
         <v>690382</v>
       </c>
@@ -17284,14 +17360,14 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="36"/>
-      <c r="C12" s="249" t="s">
+      <c r="C12" s="252" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="249"/>
-      <c r="E12" s="185">
+      <c r="D12" s="252"/>
+      <c r="E12" s="184">
         <v>0.8</v>
       </c>
-      <c r="F12" s="185">
+      <c r="F12" s="184">
         <v>0.2</v>
       </c>
       <c r="G12" s="41">
@@ -17310,14 +17386,14 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="36"/>
-      <c r="C13" s="249" t="s">
+      <c r="C13" s="252" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="249"/>
-      <c r="E13" s="250" t="s">
+      <c r="D13" s="252"/>
+      <c r="E13" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F13" s="250"/>
+      <c r="F13" s="255"/>
       <c r="G13" s="41">
         <v>1092513</v>
       </c>
@@ -17334,14 +17410,14 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="36"/>
-      <c r="C14" s="249" t="s">
+      <c r="C14" s="252" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="249"/>
-      <c r="E14" s="250" t="s">
+      <c r="D14" s="252"/>
+      <c r="E14" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F14" s="250"/>
+      <c r="F14" s="255"/>
       <c r="G14" s="41">
         <v>904227</v>
       </c>
@@ -17358,14 +17434,14 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="36"/>
-      <c r="C15" s="249" t="s">
+      <c r="C15" s="252" t="s">
         <v>300</v>
       </c>
-      <c r="D15" s="249"/>
-      <c r="E15" s="250" t="s">
+      <c r="D15" s="252"/>
+      <c r="E15" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F15" s="250"/>
+      <c r="F15" s="255"/>
       <c r="G15" s="41">
         <v>78457</v>
       </c>
@@ -17379,18 +17455,18 @@
         <v>12</v>
       </c>
       <c r="K15" s="37"/>
-      <c r="P15" s="187"/>
+      <c r="P15" s="186"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="36"/>
-      <c r="C16" s="249" t="s">
+      <c r="C16" s="252" t="s">
         <v>301</v>
       </c>
-      <c r="D16" s="249"/>
-      <c r="E16" s="185">
+      <c r="D16" s="252"/>
+      <c r="E16" s="184">
         <v>0.3</v>
       </c>
-      <c r="F16" s="185">
+      <c r="F16" s="184">
         <v>0.7</v>
       </c>
       <c r="G16" s="41">
@@ -17413,10 +17489,10 @@
         <v>302</v>
       </c>
       <c r="D17" s="251"/>
-      <c r="E17" s="185">
+      <c r="E17" s="184">
         <v>0.7</v>
       </c>
-      <c r="F17" s="185">
+      <c r="F17" s="184">
         <v>0.3</v>
       </c>
       <c r="G17" s="41">
@@ -17439,10 +17515,10 @@
         <v>25</v>
       </c>
       <c r="D18" s="251"/>
-      <c r="E18" s="250" t="s">
+      <c r="E18" s="255" t="s">
         <v>298</v>
       </c>
-      <c r="F18" s="250"/>
+      <c r="F18" s="255"/>
       <c r="G18" s="41" t="s">
         <v>299</v>
       </c>
@@ -17459,14 +17535,14 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="36"/>
-      <c r="C19" s="249" t="s">
+      <c r="C19" s="252" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="249"/>
-      <c r="E19" s="185">
+      <c r="D19" s="252"/>
+      <c r="E19" s="184">
         <v>0.47</v>
       </c>
-      <c r="F19" s="185">
+      <c r="F19" s="184">
         <v>0.53</v>
       </c>
       <c r="G19" s="41">
@@ -17485,14 +17561,14 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="36"/>
-      <c r="C20" s="249" t="s">
+      <c r="C20" s="252" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="249"/>
-      <c r="E20" s="185">
+      <c r="D20" s="252"/>
+      <c r="E20" s="184">
         <v>0.85</v>
       </c>
-      <c r="F20" s="185">
+      <c r="F20" s="184">
         <v>0.15</v>
       </c>
       <c r="G20" s="41">
@@ -17515,10 +17591,10 @@
         <v>34</v>
       </c>
       <c r="D21" s="251"/>
-      <c r="E21" s="250" t="s">
+      <c r="E21" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F21" s="250"/>
+      <c r="F21" s="255"/>
       <c r="G21" s="41">
         <v>720000</v>
       </c>
@@ -17535,14 +17611,14 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="36"/>
-      <c r="C22" s="252" t="s">
+      <c r="C22" s="256" t="s">
         <v>315</v>
       </c>
-      <c r="D22" s="253"/>
-      <c r="E22" s="250" t="s">
+      <c r="D22" s="257"/>
+      <c r="E22" s="255" t="s">
         <v>185</v>
       </c>
-      <c r="F22" s="250"/>
+      <c r="F22" s="255"/>
       <c r="G22" s="41">
         <v>300000</v>
       </c>
@@ -17559,14 +17635,14 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="36"/>
-      <c r="C23" s="249" t="s">
+      <c r="C23" s="252" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="249"/>
-      <c r="E23" s="185">
+      <c r="D23" s="252"/>
+      <c r="E23" s="184">
         <v>0.7</v>
       </c>
-      <c r="F23" s="185">
+      <c r="F23" s="184">
         <v>0.3</v>
       </c>
       <c r="G23" s="41">
@@ -17611,28 +17687,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
     <mergeCell ref="G25:K25"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E22:F22"/>
@@ -17640,6 +17694,28 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8:D8" r:id="rId1" display="750g"/>
@@ -17702,7 +17778,7 @@
     </row>
     <row r="5" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="36"/>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="131" t="s">
         <v>314</v>
       </c>
       <c r="D5" s="120" t="s">
@@ -17858,7 +17934,7 @@
       <c r="F17" s="37"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="152" t="s">
+      <c r="B18" s="151" t="s">
         <v>306</v>
       </c>
       <c r="C18" s="10"/>
@@ -17952,7 +18028,7 @@
     </row>
     <row r="6" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36"/>
-      <c r="C6" s="138" t="s">
+      <c r="C6" s="137" t="s">
         <v>114</v>
       </c>
       <c r="D6" s="120" t="s">
@@ -17980,77 +18056,77 @@
     </row>
     <row r="8" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="36"/>
-      <c r="C8" s="274"/>
-      <c r="D8" s="266" t="s">
+      <c r="C8" s="258"/>
+      <c r="D8" s="262" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="171" t="s">
+      <c r="E8" s="170" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="172">
+      <c r="F8" s="171">
         <v>42661260</v>
       </c>
-      <c r="G8" s="267">
+      <c r="G8" s="263">
         <v>12</v>
       </c>
       <c r="H8" s="37"/>
     </row>
     <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="36"/>
-      <c r="C9" s="274"/>
-      <c r="D9" s="266"/>
-      <c r="E9" s="173" t="s">
+      <c r="C9" s="258"/>
+      <c r="D9" s="262"/>
+      <c r="E9" s="172" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="173">
+      <c r="F9" s="172">
         <v>50470671</v>
       </c>
-      <c r="G9" s="268"/>
+      <c r="G9" s="264"/>
       <c r="H9" s="37"/>
     </row>
     <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="36"/>
-      <c r="C10" s="274"/>
-      <c r="D10" s="266"/>
-      <c r="E10" s="174" t="s">
+      <c r="C10" s="258"/>
+      <c r="D10" s="262"/>
+      <c r="E10" s="173" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="174">
+      <c r="F10" s="173">
         <v>3492535</v>
       </c>
-      <c r="G10" s="268"/>
+      <c r="G10" s="264"/>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="36"/>
-      <c r="C11" s="274"/>
-      <c r="D11" s="130" t="s">
+      <c r="C11" s="258"/>
+      <c r="D11" s="129" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="49" t="s">
         <v>252</v>
       </c>
-      <c r="F11" s="131">
+      <c r="F11" s="130">
         <v>93131931</v>
       </c>
-      <c r="G11" s="181">
+      <c r="G11" s="180">
         <v>16</v>
       </c>
       <c r="H11" s="37"/>
     </row>
     <row r="12" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="36"/>
-      <c r="C12" s="274"/>
-      <c r="D12" s="266" t="s">
+      <c r="C12" s="258"/>
+      <c r="D12" s="262" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="153" t="s">
+      <c r="E12" s="152" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="153">
+      <c r="F12" s="152">
         <v>35697604</v>
       </c>
-      <c r="G12" s="269">
+      <c r="G12" s="265">
         <v>14</v>
       </c>
       <c r="H12" s="37"/>
@@ -18058,45 +18134,45 @@
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="36"/>
-      <c r="C13" s="274"/>
-      <c r="D13" s="266"/>
-      <c r="E13" s="154" t="s">
+      <c r="C13" s="258"/>
+      <c r="D13" s="262"/>
+      <c r="E13" s="153" t="s">
         <v>253</v>
       </c>
-      <c r="F13" s="154">
+      <c r="F13" s="153">
         <v>16294542</v>
       </c>
-      <c r="G13" s="269"/>
+      <c r="G13" s="265"/>
       <c r="H13" s="37"/>
     </row>
     <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="36"/>
-      <c r="C14" s="274"/>
-      <c r="D14" s="270" t="s">
+      <c r="C14" s="258"/>
+      <c r="D14" s="260" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="155" t="s">
+      <c r="E14" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="F14" s="157">
+      <c r="F14" s="156">
         <v>1301100</v>
       </c>
-      <c r="G14" s="162">
+      <c r="G14" s="161">
         <v>25</v>
       </c>
       <c r="H14" s="47"/>
     </row>
     <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="36"/>
-      <c r="C15" s="274"/>
-      <c r="D15" s="270"/>
-      <c r="E15" s="156" t="s">
+      <c r="C15" s="258"/>
+      <c r="D15" s="260"/>
+      <c r="E15" s="155" t="s">
         <v>254</v>
       </c>
-      <c r="F15" s="158">
+      <c r="F15" s="157">
         <v>10330860</v>
       </c>
-      <c r="G15" s="163">
+      <c r="G15" s="162">
         <v>18</v>
       </c>
       <c r="H15" s="37"/>
@@ -18107,84 +18183,84 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="164"/>
+      <c r="G16" s="163"/>
       <c r="H16" s="37"/>
     </row>
     <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="36"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="271" t="s">
+      <c r="C17" s="168"/>
+      <c r="D17" s="266" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="175" t="s">
+      <c r="E17" s="174" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="172">
+      <c r="F17" s="171">
         <v>259383450</v>
       </c>
-      <c r="G17" s="261">
+      <c r="G17" s="272">
         <v>10</v>
       </c>
       <c r="H17" s="37"/>
     </row>
     <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="36"/>
-      <c r="C18" s="170"/>
-      <c r="D18" s="272"/>
-      <c r="E18" s="176" t="s">
+      <c r="C18" s="169"/>
+      <c r="D18" s="267"/>
+      <c r="E18" s="175" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="173">
+      <c r="F18" s="172">
         <v>11871594</v>
       </c>
-      <c r="G18" s="262"/>
+      <c r="G18" s="273"/>
       <c r="H18" s="37"/>
     </row>
     <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="36"/>
-      <c r="C19" s="167"/>
-      <c r="D19" s="272"/>
-      <c r="E19" s="176" t="s">
+      <c r="C19" s="166"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="173">
+      <c r="F19" s="172">
         <v>3960543</v>
       </c>
-      <c r="G19" s="262"/>
+      <c r="G19" s="273"/>
       <c r="H19" s="37"/>
     </row>
     <row r="20" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="36"/>
-      <c r="C20" s="179"/>
-      <c r="D20" s="273"/>
-      <c r="E20" s="177" t="s">
+      <c r="C20" s="178"/>
+      <c r="D20" s="268"/>
+      <c r="E20" s="176" t="s">
         <v>118</v>
       </c>
-      <c r="F20" s="174">
+      <c r="F20" s="173">
         <v>770703</v>
       </c>
-      <c r="G20" s="262"/>
+      <c r="G20" s="273"/>
       <c r="H20" s="37"/>
     </row>
     <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="36"/>
-      <c r="C21" s="179"/>
-      <c r="D21" s="180" t="s">
+      <c r="C21" s="178"/>
+      <c r="D21" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="177" t="s">
+      <c r="E21" s="176" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="174">
+      <c r="F21" s="173">
         <v>29946799</v>
       </c>
-      <c r="G21" s="263"/>
+      <c r="G21" s="274"/>
       <c r="H21" s="37"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="36"/>
-      <c r="C22" s="168"/>
-      <c r="D22" s="166" t="s">
+      <c r="C22" s="167"/>
+      <c r="D22" s="165" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="49" t="s">
@@ -18193,7 +18269,7 @@
       <c r="F22" s="48">
         <v>323000000</v>
       </c>
-      <c r="G22" s="165">
+      <c r="G22" s="164">
         <v>14</v>
       </c>
       <c r="H22" s="37"/>
@@ -18204,102 +18280,102 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="164"/>
+      <c r="G23" s="163"/>
       <c r="H23" s="37"/>
     </row>
     <row r="24" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="36"/>
-      <c r="C24" s="275"/>
-      <c r="D24" s="270" t="s">
+      <c r="C24" s="259"/>
+      <c r="D24" s="260" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="153" t="s">
+      <c r="E24" s="152" t="s">
         <v>116</v>
       </c>
-      <c r="F24" s="153">
+      <c r="F24" s="152">
         <v>32351408</v>
       </c>
-      <c r="G24" s="265">
+      <c r="G24" s="276">
         <v>8</v>
       </c>
       <c r="H24" s="37"/>
     </row>
     <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="36"/>
-      <c r="C25" s="275"/>
-      <c r="D25" s="270"/>
-      <c r="E25" s="159" t="s">
+      <c r="C25" s="259"/>
+      <c r="D25" s="260"/>
+      <c r="E25" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="F25" s="160">
+      <c r="F25" s="159">
         <v>12752184</v>
       </c>
-      <c r="G25" s="265"/>
+      <c r="G25" s="276"/>
       <c r="H25" s="37"/>
     </row>
     <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="36"/>
-      <c r="C26" s="275"/>
-      <c r="D26" s="270"/>
-      <c r="E26" s="159" t="s">
+      <c r="C26" s="259"/>
+      <c r="D26" s="260"/>
+      <c r="E26" s="158" t="s">
         <v>118</v>
       </c>
-      <c r="F26" s="160">
+      <c r="F26" s="159">
         <v>13211821</v>
       </c>
-      <c r="G26" s="265"/>
+      <c r="G26" s="276"/>
       <c r="H26" s="37"/>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="36"/>
-      <c r="C27" s="275"/>
-      <c r="D27" s="270"/>
-      <c r="E27" s="159" t="s">
+      <c r="C27" s="259"/>
+      <c r="D27" s="260"/>
+      <c r="E27" s="158" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="160">
+      <c r="F27" s="159">
         <v>4050471</v>
       </c>
-      <c r="G27" s="265"/>
+      <c r="G27" s="276"/>
       <c r="H27" s="37"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="36"/>
-      <c r="C28" s="275"/>
-      <c r="D28" s="270"/>
-      <c r="E28" s="161" t="s">
+      <c r="C28" s="259"/>
+      <c r="D28" s="260"/>
+      <c r="E28" s="160" t="s">
         <v>119</v>
       </c>
-      <c r="F28" s="154">
+      <c r="F28" s="153">
         <v>14771946</v>
       </c>
-      <c r="G28" s="265"/>
+      <c r="G28" s="276"/>
       <c r="H28" s="37"/>
     </row>
     <row r="29" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="36"/>
-      <c r="C29" s="275"/>
-      <c r="D29" s="270" t="s">
+      <c r="C29" s="259"/>
+      <c r="D29" s="260" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="276" t="s">
+      <c r="E29" s="261" t="s">
         <v>122</v>
       </c>
-      <c r="F29" s="264">
+      <c r="F29" s="275">
         <v>77137830</v>
       </c>
-      <c r="G29" s="265">
+      <c r="G29" s="276">
         <v>12</v>
       </c>
       <c r="H29" s="37"/>
     </row>
     <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="36"/>
-      <c r="C30" s="275"/>
-      <c r="D30" s="270"/>
-      <c r="E30" s="276"/>
-      <c r="F30" s="264"/>
-      <c r="G30" s="265"/>
+      <c r="C30" s="259"/>
+      <c r="D30" s="260"/>
+      <c r="E30" s="261"/>
+      <c r="F30" s="275"/>
+      <c r="G30" s="276"/>
       <c r="H30" s="37"/>
     </row>
     <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18308,76 +18384,76 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="164"/>
+      <c r="G31" s="163"/>
       <c r="H31" s="37"/>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="36"/>
-      <c r="C32" s="258"/>
-      <c r="D32" s="271" t="s">
+      <c r="C32" s="269"/>
+      <c r="D32" s="266" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="178" t="s">
+      <c r="E32" s="177" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="153">
+      <c r="F32" s="152">
         <v>18205094</v>
       </c>
-      <c r="G32" s="261">
+      <c r="G32" s="272">
         <v>5</v>
       </c>
       <c r="H32" s="37"/>
     </row>
     <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="36"/>
-      <c r="C33" s="259"/>
-      <c r="D33" s="272"/>
-      <c r="E33" s="176" t="s">
+      <c r="C33" s="270"/>
+      <c r="D33" s="267"/>
+      <c r="E33" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="160">
+      <c r="F33" s="159">
         <v>19747877</v>
       </c>
-      <c r="G33" s="262"/>
+      <c r="G33" s="273"/>
       <c r="H33" s="37"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="36"/>
-      <c r="C34" s="259"/>
-      <c r="D34" s="272"/>
-      <c r="E34" s="176" t="s">
+      <c r="C34" s="270"/>
+      <c r="D34" s="267"/>
+      <c r="E34" s="175" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="160">
+      <c r="F34" s="159">
         <v>1765305</v>
       </c>
-      <c r="G34" s="262"/>
+      <c r="G34" s="273"/>
       <c r="H34" s="37"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="36"/>
-      <c r="C35" s="259"/>
-      <c r="D35" s="272"/>
-      <c r="E35" s="176" t="s">
+      <c r="C35" s="270"/>
+      <c r="D35" s="267"/>
+      <c r="E35" s="175" t="s">
         <v>116</v>
       </c>
-      <c r="F35" s="160">
+      <c r="F35" s="159">
         <v>26650077</v>
       </c>
-      <c r="G35" s="262"/>
+      <c r="G35" s="273"/>
       <c r="H35" s="37"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
-      <c r="C36" s="260"/>
-      <c r="D36" s="273"/>
-      <c r="E36" s="177" t="s">
+      <c r="C36" s="271"/>
+      <c r="D36" s="268"/>
+      <c r="E36" s="176" t="s">
         <v>119</v>
       </c>
-      <c r="F36" s="154">
+      <c r="F36" s="153">
         <v>4506444</v>
       </c>
-      <c r="G36" s="263"/>
+      <c r="G36" s="274"/>
       <c r="H36" s="37"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -18402,11 +18478,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C8:C15"/>
-    <mergeCell ref="C24:C30"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="G32:G36"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="G24:G28"/>
     <mergeCell ref="E38:H38"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="G8:G10"/>
@@ -18415,12 +18492,11 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D32:D36"/>
     <mergeCell ref="D17:D20"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -18478,69 +18554,69 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
-      <c r="B5" s="136"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="123" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="137"/>
+      <c r="D5" s="136"/>
       <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
-      <c r="B6" s="133" t="s">
+      <c r="B6" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="133" t="s">
         <v>226</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="134" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
-      <c r="B7" s="279"/>
+      <c r="B7" s="277"/>
       <c r="C7" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="279"/>
+      <c r="D7" s="277"/>
       <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
-      <c r="B8" s="280"/>
+      <c r="B8" s="278"/>
       <c r="C8" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="280"/>
+      <c r="D8" s="278"/>
       <c r="E8" s="37"/>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
-      <c r="B9" s="280"/>
+      <c r="B9" s="278"/>
       <c r="C9" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="280"/>
+      <c r="D9" s="278"/>
       <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
-      <c r="B10" s="280"/>
+      <c r="B10" s="278"/>
       <c r="C10" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="280"/>
+      <c r="D10" s="278"/>
       <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
-      <c r="B11" s="278"/>
+      <c r="B11" s="279"/>
       <c r="C11" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="278"/>
+      <c r="D11" s="279"/>
       <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18552,25 +18628,25 @@
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36"/>
-      <c r="B13" s="281" t="s">
+      <c r="B13" s="280" t="s">
         <v>265</v>
       </c>
-      <c r="C13" s="282"/>
-      <c r="D13" s="283"/>
+      <c r="C13" s="281"/>
+      <c r="D13" s="282"/>
       <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
-      <c r="B14" s="277"/>
-      <c r="C14" s="277"/>
-      <c r="D14" s="128"/>
+      <c r="B14" s="283"/>
+      <c r="C14" s="283"/>
+      <c r="D14" s="127"/>
       <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
-      <c r="B15" s="278"/>
-      <c r="C15" s="278"/>
-      <c r="D15" s="129"/>
+      <c r="B15" s="279"/>
+      <c r="C15" s="279"/>
+      <c r="D15" s="128"/>
       <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18588,16 +18664,16 @@
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
-      <c r="B17" s="277"/>
-      <c r="C17" s="277"/>
-      <c r="D17" s="128"/>
+      <c r="B17" s="283"/>
+      <c r="C17" s="283"/>
+      <c r="D17" s="127"/>
       <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
-      <c r="B18" s="278"/>
-      <c r="C18" s="278"/>
-      <c r="D18" s="129"/>
+      <c r="B18" s="279"/>
+      <c r="C18" s="279"/>
+      <c r="D18" s="128"/>
       <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18615,16 +18691,16 @@
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
-      <c r="B20" s="277"/>
-      <c r="C20" s="277"/>
-      <c r="D20" s="128"/>
+      <c r="B20" s="283"/>
+      <c r="C20" s="283"/>
+      <c r="D20" s="127"/>
       <c r="E20" s="37"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
-      <c r="B21" s="278"/>
-      <c r="C21" s="278"/>
-      <c r="D21" s="129"/>
+      <c r="B21" s="279"/>
+      <c r="C21" s="279"/>
+      <c r="D21" s="128"/>
       <c r="E21" s="37"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18649,10 +18725,10 @@
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="137" t="s">
         <v>257</v>
       </c>
-      <c r="C24" s="139" t="s">
+      <c r="C24" s="138" t="s">
         <v>142</v>
       </c>
       <c r="D24" s="23"/>
@@ -18711,16 +18787,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -18797,22 +18873,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
-      <c r="B6" s="284"/>
-      <c r="C6" s="277"/>
-      <c r="D6" s="277"/>
-      <c r="E6" s="277"/>
-      <c r="F6" s="277"/>
-      <c r="G6" s="286"/>
+      <c r="B6" s="286"/>
+      <c r="C6" s="283"/>
+      <c r="D6" s="283"/>
+      <c r="E6" s="283"/>
+      <c r="F6" s="283"/>
+      <c r="G6" s="284"/>
       <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
-      <c r="B7" s="285"/>
-      <c r="C7" s="278"/>
-      <c r="D7" s="278"/>
-      <c r="E7" s="278"/>
-      <c r="F7" s="278"/>
-      <c r="G7" s="287"/>
+      <c r="B7" s="287"/>
+      <c r="C7" s="279"/>
+      <c r="D7" s="279"/>
+      <c r="E7" s="279"/>
+      <c r="F7" s="279"/>
+      <c r="G7" s="285"/>
       <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18849,22 +18925,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
-      <c r="B10" s="284"/>
-      <c r="C10" s="277"/>
-      <c r="D10" s="277"/>
-      <c r="E10" s="277"/>
-      <c r="F10" s="277"/>
-      <c r="G10" s="286"/>
+      <c r="B10" s="286"/>
+      <c r="C10" s="283"/>
+      <c r="D10" s="283"/>
+      <c r="E10" s="283"/>
+      <c r="F10" s="283"/>
+      <c r="G10" s="284"/>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
-      <c r="B11" s="285"/>
-      <c r="C11" s="278"/>
-      <c r="D11" s="278"/>
-      <c r="E11" s="278"/>
-      <c r="F11" s="278"/>
-      <c r="G11" s="287"/>
+      <c r="B11" s="287"/>
+      <c r="C11" s="279"/>
+      <c r="D11" s="279"/>
+      <c r="E11" s="279"/>
+      <c r="F11" s="279"/>
+      <c r="G11" s="285"/>
       <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18901,22 +18977,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
-      <c r="B14" s="284"/>
-      <c r="C14" s="277"/>
-      <c r="D14" s="277"/>
-      <c r="E14" s="277"/>
-      <c r="F14" s="277"/>
-      <c r="G14" s="286"/>
+      <c r="B14" s="286"/>
+      <c r="C14" s="283"/>
+      <c r="D14" s="283"/>
+      <c r="E14" s="283"/>
+      <c r="F14" s="283"/>
+      <c r="G14" s="284"/>
       <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
-      <c r="B15" s="285"/>
-      <c r="C15" s="278"/>
-      <c r="D15" s="278"/>
-      <c r="E15" s="278"/>
-      <c r="F15" s="278"/>
-      <c r="G15" s="287"/>
+      <c r="B15" s="287"/>
+      <c r="C15" s="279"/>
+      <c r="D15" s="279"/>
+      <c r="E15" s="279"/>
+      <c r="F15" s="279"/>
+      <c r="G15" s="285"/>
       <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18953,22 +19029,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
-      <c r="B18" s="284"/>
-      <c r="C18" s="277"/>
-      <c r="D18" s="277"/>
-      <c r="E18" s="277"/>
-      <c r="F18" s="277"/>
-      <c r="G18" s="286"/>
+      <c r="B18" s="286"/>
+      <c r="C18" s="283"/>
+      <c r="D18" s="283"/>
+      <c r="E18" s="283"/>
+      <c r="F18" s="283"/>
+      <c r="G18" s="284"/>
       <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
-      <c r="B19" s="285"/>
-      <c r="C19" s="278"/>
-      <c r="D19" s="278"/>
-      <c r="E19" s="278"/>
-      <c r="F19" s="278"/>
-      <c r="G19" s="287"/>
+      <c r="B19" s="287"/>
+      <c r="C19" s="279"/>
+      <c r="D19" s="279"/>
+      <c r="E19" s="279"/>
+      <c r="F19" s="279"/>
+      <c r="G19" s="285"/>
       <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19051,6 +19127,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="F18:F19"/>
@@ -19060,22 +19152,6 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>